<commit_message>
* Added the key layout. * Join columns are not mandatory anymore. * Functions dumping the values to the output are renamed to dump*. * Added the information about data source to header columns in normal, interlaced and key layouts. * Other code re-factoring.
</commit_message>
<xml_diff>
--- a/tests/data/desired/excludecolumnsreport.xlsx
+++ b/tests/data/desired/excludecolumnsreport.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -46,7 +46,10 @@
     <t>Abone8</t>
   </si>
   <si>
-    <t>FIRST_NAME</t>
+    <t>FIRST_NAME (Source1)</t>
+  </si>
+  <si>
+    <t>FIRST_NAME (Source2)</t>
   </si>
   <si>
     <t>1Martin1</t>
@@ -194,7 +197,7 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
@@ -202,10 +205,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -213,10 +216,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -224,10 +227,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -235,10 +238,10 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
@@ -246,10 +249,10 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
@@ -257,10 +260,10 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Adding the number of differences to every row in normal and interlaced layouts. * Adding the location information to the parser error into the log. * Removing the parser exception dump as the error message is sufficient.
</commit_message>
<xml_diff>
--- a/tests/data/desired/excludecolumnsreport.xlsx
+++ b/tests/data/desired/excludecolumnsreport.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Abone8</t>
+  </si>
+  <si>
+    <t># of Diffs</t>
   </si>
   <si>
     <t>FIRST_NAME (Source1)</t>
@@ -191,79 +194,100 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>10</v>
       </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="s" s="1">
-        <v>11</v>
+      <c r="A2" t="n" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.0</v>
       </c>
       <c r="C2" t="s" s="1">
         <v>12</v>
       </c>
+      <c r="D2" t="s" s="1">
+        <v>13</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="n" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B3" t="n">
         <v>2.0</v>
-      </c>
-      <c r="B3" t="s" s="1">
-        <v>13</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>14</v>
       </c>
+      <c r="D3" t="s" s="1">
+        <v>15</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="n">
         <v>3.0</v>
-      </c>
-      <c r="B4" t="s" s="1">
-        <v>15</v>
       </c>
       <c r="C4" t="s" s="1">
         <v>16</v>
       </c>
+      <c r="D4" t="s" s="1">
+        <v>17</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B5" t="n">
         <v>4.0</v>
-      </c>
-      <c r="B5" t="s" s="1">
-        <v>16</v>
       </c>
       <c r="C5" t="s" s="1">
         <v>17</v>
       </c>
+      <c r="D5" t="s" s="1">
+        <v>18</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B6" t="n">
         <v>5.0</v>
       </c>
-      <c r="B6" t="s" s="1">
-        <v>18</v>
-      </c>
       <c r="C6" t="s" s="1">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="D6" t="s" s="1">
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B7" t="n">
         <v>6.0</v>
       </c>
-      <c r="B7" t="s" s="1">
-        <v>16</v>
-      </c>
       <c r="C7" t="s" s="1">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="D7" t="s" s="1">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Optimization of cell style work.
</commit_message>
<xml_diff>
--- a/tests/data/desired/excludecolumnsreport.xlsx
+++ b/tests/data/desired/excludecolumnsreport.xlsx
@@ -89,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -111,18 +111,37 @@
       <sz val="10"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="D02020"/>
-      <u val="none"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -157,14 +176,13 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+  <cellXfs count="4">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -193,100 +211,100 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="2">
         <v>11</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C2" t="s" s="1">
+      <c r="A2" t="n" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="n" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="C2" t="s" s="3">
         <v>12</v>
       </c>
-      <c r="D2" t="s" s="1">
+      <c r="D2" t="s" s="3">
         <v>13</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B3" t="n">
+      <c r="A3" t="n" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B3" t="n" s="2">
         <v>2.0</v>
       </c>
-      <c r="C3" t="s" s="1">
+      <c r="C3" t="s" s="3">
         <v>14</v>
       </c>
-      <c r="D3" t="s" s="1">
+      <c r="D3" t="s" s="3">
         <v>15</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B4" t="n" s="1">
+      <c r="A4" t="n" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="n" s="3">
         <v>3.0</v>
       </c>
-      <c r="C4" t="s" s="1">
+      <c r="C4" t="s" s="3">
         <v>16</v>
       </c>
-      <c r="D4" t="s" s="1">
+      <c r="D4" t="s" s="3">
         <v>17</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B5" t="n" s="1">
+      <c r="A5" t="n" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B5" t="n" s="3">
         <v>4.0</v>
       </c>
-      <c r="C5" t="s" s="1">
+      <c r="C5" t="s" s="3">
         <v>17</v>
       </c>
-      <c r="D5" t="s" s="1">
+      <c r="D5" t="s" s="3">
         <v>18</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B6" t="n" s="1">
+      <c r="A6" t="n" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B6" t="n" s="3">
         <v>5.0</v>
       </c>
-      <c r="C6" t="s" s="1">
+      <c r="C6" t="s" s="3">
         <v>19</v>
       </c>
-      <c r="D6" t="s" s="1">
+      <c r="D6" t="s" s="3">
         <v>17</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B7" t="n" s="1">
+      <c r="A7" t="n" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B7" t="n" s="3">
         <v>6.0</v>
       </c>
-      <c r="C7" t="s" s="1">
+      <c r="C7" t="s" s="3">
         <v>17</v>
       </c>
-      <c r="D7" t="s" s="1">
+      <c r="D7" t="s" s="3">
         <v>20</v>
       </c>
     </row>
@@ -317,79 +335,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" t="n" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="n" s="1">
         <v>11.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="n" s="1">
         <v>2.0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="1">
         <v>4</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="n" s="1">
         <v>12.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" t="n" s="1">
         <v>3.0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="1">
         <v>5</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" t="n" s="1">
         <v>13.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="n" s="1">
         <v>5.0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="1">
         <v>6</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" t="n" s="1">
         <v>15.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="n" s="1">
         <v>7.0</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="1">
         <v>7</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" t="n" s="1">
         <v>77.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" t="n" s="1">
         <v>8.0</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="1">
         <v>8</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" t="n" s="1">
         <v>15.0</v>
       </c>
     </row>

</xml_diff>